<commit_message>
Add check of student_intensive_lectures' validation
</commit_message>
<xml_diff>
--- a/public/講義登録_テンプレート.xlsx
+++ b/public/講義登録_テンプレート.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,42 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>ここに、LiveCampusからコピーした個人時間割を貼り付けてください。</t>
+    <rPh sb="21" eb="23">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="23" eb="26">
+      <t>ジカンワリ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ハ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,11 +77,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -335,8 +366,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="90">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>